<commit_message>
Added MySQL Data Warehouse Script
</commit_message>
<xml_diff>
--- a/Documentation/DimensionModel.xlsx
+++ b/Documentation/DimensionModel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dimensions" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>PermNum</t>
   </si>
   <si>
-    <t>Middle_Name</t>
-  </si>
-  <si>
     <t>Generation</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>IEPDate</t>
   </si>
   <si>
-    <t>ClassAffiliateID</t>
-  </si>
-  <si>
     <t>ClassAffiliate</t>
   </si>
   <si>
@@ -301,24 +295,12 @@
     <t>DayName</t>
   </si>
   <si>
-    <t>Dow</t>
-  </si>
-  <si>
-    <t>DowNum</t>
-  </si>
-  <si>
-    <t>Doy</t>
-  </si>
-  <si>
     <t>WeekId</t>
   </si>
   <si>
     <t>WeekName</t>
   </si>
   <si>
-    <t>Woy</t>
-  </si>
-  <si>
     <t>WeekStart</t>
   </si>
   <si>
@@ -506,6 +488,24 @@
   </si>
   <si>
     <t>ExpulsionServiceFlag</t>
+  </si>
+  <si>
+    <t>ClassAffiliateId</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOW </t>
+  </si>
+  <si>
+    <t>DOWNum</t>
+  </si>
+  <si>
+    <t>DOY</t>
+  </si>
+  <si>
+    <t>WOY</t>
   </si>
 </sst>
 </file>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,19 +947,19 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="K3" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="P3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -979,10 +979,10 @@
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="H4" s="2">
         <v>10</v>
@@ -991,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -1003,7 +1003,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -1029,7 +1029,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>3</v>
@@ -1041,7 +1041,7 @@
         <v>6</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>3</v>
@@ -1053,10 +1053,10 @@
         <v>6</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2" t="s">
@@ -1077,7 +1077,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>3</v>
@@ -1089,10 +1089,10 @@
         <v>6</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M6" s="2">
         <v>3</v>
@@ -1101,7 +1101,7 @@
         <v>6</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>3</v>
@@ -1127,7 +1127,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>3</v>
@@ -1139,10 +1139,10 @@
         <v>6</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M7" s="2">
         <v>30</v>
@@ -1151,7 +1151,7 @@
         <v>6</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>3</v>
@@ -1177,10 +1177,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="2">
         <v>50</v>
@@ -1189,10 +1189,10 @@
         <v>6</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M8" s="2">
         <v>3</v>
@@ -1201,10 +1201,10 @@
         <v>6</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R8" s="2">
         <v>4</v>
@@ -1215,10 +1215,10 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2">
         <v>50</v>
@@ -1227,10 +1227,10 @@
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="2">
         <v>50</v>
@@ -1239,10 +1239,10 @@
         <v>6</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9" s="2">
         <v>20</v>
@@ -1251,10 +1251,10 @@
         <v>6</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2" t="s">
@@ -1263,10 +1263,10 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2">
         <v>50</v>
@@ -1275,10 +1275,10 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="2">
         <v>50</v>
@@ -1287,10 +1287,10 @@
         <v>6</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" s="3">
         <v>20</v>
@@ -1299,10 +1299,10 @@
         <v>6</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2" t="s">
@@ -1311,10 +1311,10 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -1323,10 +1323,10 @@
         <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" s="2">
         <v>1</v>
@@ -1335,17 +1335,17 @@
         <v>6</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>3</v>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2">
         <v>10</v>
@@ -1371,10 +1371,10 @@
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H12" s="2">
         <v>2</v>
@@ -1383,20 +1383,20 @@
         <v>6</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R12" s="2">
         <v>7</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
@@ -1419,10 +1419,10 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="2">
         <v>50</v>
@@ -1431,7 +1431,7 @@
         <v>6</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>3</v>
@@ -1445,10 +1445,10 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2">
         <v>20</v>
@@ -1457,10 +1457,10 @@
         <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" s="2">
         <v>100</v>
@@ -1469,10 +1469,10 @@
         <v>6</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R14" s="2">
         <v>7</v>
@@ -1483,20 +1483,20 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="2">
         <v>20</v>
@@ -1505,10 +1505,10 @@
         <v>6</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2" t="s">
@@ -1517,20 +1517,20 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16" s="2">
         <v>2</v>
@@ -1539,10 +1539,10 @@
         <v>6</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="2" t="s">
@@ -1551,7 +1551,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>156</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
@@ -1563,10 +1563,10 @@
         <v>6</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17" s="2">
         <v>5</v>
@@ -1575,7 +1575,7 @@
         <v>6</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>3</v>
@@ -1589,10 +1589,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2">
         <v>50</v>
@@ -1601,10 +1601,10 @@
         <v>6</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="2">
         <v>30</v>
@@ -1613,10 +1613,10 @@
         <v>6</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R18" s="2">
         <v>6</v>
@@ -1627,10 +1627,10 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -1639,10 +1639,10 @@
         <v>6</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" s="2">
         <v>30</v>
@@ -1651,7 +1651,7 @@
         <v>6</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>3</v>
@@ -1665,10 +1665,10 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="3">
         <v>20</v>
@@ -1677,10 +1677,10 @@
         <v>6</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" s="2">
         <v>30</v>
@@ -1689,7 +1689,7 @@
         <v>6</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>3</v>
@@ -1703,17 +1703,17 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>3</v>
@@ -1725,7 +1725,7 @@
         <v>6</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q21" s="2" t="s">
         <v>3</v>
@@ -1739,17 +1739,17 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>3</v>
@@ -1761,7 +1761,7 @@
         <v>6</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>3</v>
@@ -1775,10 +1775,10 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F23" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" s="2">
         <v>30</v>
@@ -1787,10 +1787,10 @@
         <v>6</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R23" s="2">
         <v>10</v>
@@ -1801,10 +1801,10 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24" s="2">
         <v>50</v>
@@ -1813,10 +1813,10 @@
         <v>6</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R24" s="2">
         <v>3</v>
@@ -1827,10 +1827,10 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25" s="2">
         <v>50</v>
@@ -1839,7 +1839,7 @@
         <v>6</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>3</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>3</v>
@@ -1865,7 +1865,7 @@
         <v>6</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>3</v>
@@ -1879,10 +1879,10 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F27" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" s="2">
         <v>20</v>
@@ -1891,7 +1891,7 @@
         <v>6</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="Q27" s="2" t="s">
         <v>3</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F28" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>3</v>
@@ -1917,10 +1917,10 @@
         <v>6</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R28" s="2">
         <v>20</v>
@@ -1931,10 +1931,10 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F29" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="2">
         <v>20</v>
@@ -1943,7 +1943,7 @@
         <v>6</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>98</v>
+        <v>161</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>3</v>
@@ -1957,10 +1957,10 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F30" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="2">
         <v>20</v>
@@ -1969,7 +1969,7 @@
         <v>6</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Q30" s="2" t="s">
         <v>3</v>
@@ -1983,10 +1983,10 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F31" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H31" s="2">
         <v>20</v>
@@ -1995,7 +1995,7 @@
         <v>6</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>3</v>
@@ -2009,7 +2009,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F32" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>3</v>
@@ -2021,10 +2021,10 @@
         <v>6</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R32" s="2">
         <v>4</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="33" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F33" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>3</v>
@@ -2047,10 +2047,10 @@
         <v>6</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2" t="s">
@@ -2059,10 +2059,10 @@
     </row>
     <row r="34" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F34" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H34" s="2">
         <v>20</v>
@@ -2071,10 +2071,10 @@
         <v>6</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2" t="s">
@@ -2083,20 +2083,20 @@
     </row>
     <row r="35" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F35" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R35" s="2">
         <v>7</v>
@@ -2107,20 +2107,20 @@
     </row>
     <row r="36" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F36" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R36" s="2">
         <v>7</v>
@@ -2131,20 +2131,20 @@
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F37" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R37" s="2">
         <v>6</v>
@@ -2155,10 +2155,10 @@
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F38" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H38" s="2">
         <v>2</v>
@@ -2167,7 +2167,7 @@
         <v>6</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>3</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="39" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F39" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>3</v>
@@ -2193,10 +2193,10 @@
         <v>6</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R39" s="2">
         <v>20</v>
@@ -2207,10 +2207,10 @@
     </row>
     <row r="40" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F40" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H40" s="2">
         <v>20</v>
@@ -2219,7 +2219,7 @@
         <v>6</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Q40" s="2" t="s">
         <v>3</v>
@@ -2233,17 +2233,17 @@
     </row>
     <row r="41" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F41" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>3</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="42" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F42" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>3</v>
@@ -2269,10 +2269,10 @@
         <v>6</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R42" s="2">
         <v>4</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="43" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F43" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>3</v>
@@ -2295,10 +2295,10 @@
         <v>6</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R43" s="2">
         <v>7</v>
@@ -2309,10 +2309,10 @@
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F44" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H44" s="2">
         <v>50</v>
@@ -2321,10 +2321,10 @@
         <v>6</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R44" s="2">
         <v>6</v>
@@ -2335,10 +2335,10 @@
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F45" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H45" s="3">
         <v>20</v>
@@ -2347,7 +2347,7 @@
         <v>6</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="Q45" s="2" t="s">
         <v>3</v>
@@ -2361,17 +2361,17 @@
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F46" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="3" t="s">
         <v>6</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="Q46" s="2" t="s">
         <v>3</v>
@@ -2385,20 +2385,20 @@
     </row>
     <row r="47" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F47" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="3" t="s">
         <v>9</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R47" s="2">
         <v>6</v>
@@ -2409,10 +2409,10 @@
     </row>
     <row r="48" spans="6:19" x14ac:dyDescent="0.3">
       <c r="P48" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R48" s="2">
         <v>4</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="49" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P49" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>3</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="50" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P50" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>3</v>
@@ -2451,10 +2451,10 @@
     </row>
     <row r="51" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P51" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R51" s="2">
         <v>7</v>
@@ -2465,10 +2465,10 @@
     </row>
     <row r="52" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P52" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R52" s="3">
         <v>20</v>
@@ -2479,10 +2479,10 @@
     </row>
     <row r="53" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P53" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R53" s="2"/>
       <c r="S53" s="3" t="s">
@@ -2491,10 +2491,10 @@
     </row>
     <row r="54" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P54" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="3" t="s">
@@ -2511,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2527,24 +2527,24 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="F3" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="K3" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -2552,7 +2552,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -2564,7 +2564,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>3</v>
@@ -2576,7 +2576,7 @@
         <v>4</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -2602,7 +2602,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>3</v>
@@ -2614,7 +2614,7 @@
         <v>6</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>3</v>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -2637,10 +2637,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>3</v>
@@ -2649,10 +2649,10 @@
         <v>10</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>3</v>
@@ -2661,12 +2661,12 @@
         <v>10</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -2675,10 +2675,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>3</v>
@@ -2687,10 +2687,10 @@
         <v>10</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>3</v>
@@ -2699,12 +2699,12 @@
         <v>10</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -2713,10 +2713,10 @@
         <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>3</v>
@@ -2725,10 +2725,10 @@
         <v>10</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>3</v>
@@ -2737,27 +2737,27 @@
         <v>10</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="2">
         <v>20</v>
@@ -2766,10 +2766,10 @@
         <v>6</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9" s="2">
         <v>30</v>
@@ -2780,10 +2780,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -2792,10 +2792,10 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="2">
         <v>20</v>
@@ -2804,10 +2804,10 @@
         <v>6</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2" t="s">
@@ -2816,7 +2816,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
@@ -2828,10 +2828,10 @@
         <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" s="2">
         <v>2</v>
@@ -2840,10 +2840,10 @@
         <v>6</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M11" s="3">
         <v>20</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -2866,10 +2866,10 @@
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" s="2">
         <v>20</v>
@@ -2878,10 +2878,10 @@
         <v>6</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="3" t="s">
@@ -2890,7 +2890,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
@@ -2902,20 +2902,20 @@
         <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="3" t="s">
@@ -2924,7 +2924,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
@@ -2936,7 +2936,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>3</v>
@@ -2950,20 +2950,20 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
@@ -2972,10 +2972,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="3">
         <v>20</v>
@@ -2984,7 +2984,7 @@
         <v>6</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>3</v>
@@ -2998,20 +2998,20 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" s="3">
         <v>20</v>
@@ -3022,20 +3022,20 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="3" t="s">
@@ -3044,10 +3044,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F19" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="3" t="s">

</xml_diff>

<commit_message>
Added the Talend Project
1. Added STUDENT_BEHAVIOR_DI Talend Project
2. Modified MySQL Data Warehouse
3. Modified DimensionModel.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/DimensionModel.xlsx
+++ b/Documentation/DimensionModel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="163">
   <si>
     <t>Dimensions</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>WOY</t>
+  </si>
+  <si>
+    <t>bigint</t>
   </si>
 </sst>
 </file>
@@ -916,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,10 +1095,10 @@
         <v>127</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M6" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>6</v>
@@ -1118,7 +1121,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="C7" s="2">
         <v>10</v>
@@ -1145,7 +1148,7 @@
         <v>16</v>
       </c>
       <c r="M7" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>6</v>
@@ -1192,10 +1195,10 @@
         <v>129</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M8" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>6</v>
@@ -1314,10 +1317,10 @@
         <v>157</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
@@ -1451,7 +1454,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -2511,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2707,7 +2710,7 @@
         <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="C8" s="2">
         <v>10</v>
@@ -2760,7 +2763,7 @@
         <v>16</v>
       </c>
       <c r="H9" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>6</v>
@@ -2786,7 +2789,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>

</xml_diff>